<commit_message>
Removed executorRepository, add group description in datagrid, add canExecute to command
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -32,25 +32,144 @@
   <si>
     <t>移除Programs里面不必要的event</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dash Board</t>
+  </si>
+  <si>
+    <t>Save as, edit resources</t>
+  </si>
+  <si>
+    <t>DataGrid如何分组？</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/dotnet/framework/wpf/controls/how-to-group-sort-and-filter-data-in-the-datagrid-control</t>
+  </si>
+  <si>
+    <t>DataGrid分组如何实时更新？</t>
+  </si>
+  <si>
+    <t>.Net Framework 4.0的datagrid根本就不支持实时更新Group。
+WPF在model和View之间提供了一个中间层CollectionViewSource。它在XAML中定义，其中包含一个CollectionView。CollectionView可以理解为model打包生成的ViewModel。也就是说，如果我们将model绑定到CollectionViewSource的Source属性，则WPF帮我们创建了一个ViewModel。这个ViewModel会被用来分组，排序，从而在UI上显示分组和排序后的数据。
+也就是说，WPF帮我们实现了MVVM。可是这个实现在.Net4.0还不完善，不支持Group的实时更新。
+所以，我们可以选择抛弃WPF帮我们实现的这个并不完善的DataGrid，自己来实现一个可实时分组的控件。
+也可以试试新的.Net FrameWork，4.5及以上版本已经实现了实时分组功能。</t>
+  </si>
+  <si>
+    <t>当model改变时，如何通知view改变？</t>
+  </si>
+  <si>
+    <t>如果是通过Command来修改model，那么当然可以在Viewmodel中呼叫OnPropertyChanged(propertyName)来通知view。可是如果是model自己在变呢（或者被一个外部的service改变）？看了一圈资料，貌似只能用INotifyPropertyChanged</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Later</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Command完善</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>点击Invalidate之后会为RequestedRecipe添加Executor，如何更新AllExecutorsView？</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <r>
+      <t>这个问题是item 5 的一个子集：ViewModel将model中的一个数据改了，而这个数据的改动导致model中其他数据也被改动了。这种情况下，如何更新UI？
+不同于完全由外部修改model，这个问题中，我们可以假设ViewModel“</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>知道</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>”自己的某些改动会带来某些后果，因此可以在ViewModel的层面来解决问题。（例如重新生成AllExecutors，或设法找到新的Executor然后添加到AllExecutors中来。在我们这个项目中，这两个办法要么显然不合理，要么很麻烦。）
+当然，这个“</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>知道</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>”就是耦合。如果不希望有这种程度的耦合，也可以在model上做手脚，方法不外乎以下两种：
+1. 在model中建立新的数据结构，ExecutorRepository。AddExecutor实际上是往Repository里面AddItem，那么ItemAdded事件会被viewmodel响应，从而更新UI
+2. 不加新的数据结构，而是为AddExecutor产生新的事件ExecutorAdded。ViewModel中订阅此事件，从而在响应事件时更新UI。
+显然，我们不应该为了ViewModel而去改变Model，或者说尽量少改动。所以这里方案二明显较优</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -71,17 +190,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -94,7 +227,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -168,7 +301,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -203,7 +335,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -379,58 +510,157 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="65.625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="2" max="2" width="65.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="116.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="120">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="210">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -438,12 +668,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed model-viewmodel collection operation sync issue
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -514,7 +514,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -642,6 +642,9 @@
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented save as, but the mainWindowViewModel is everywhere!
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,6 +135,41 @@
 1. 在model中建立新的数据结构，ExecutorRepository。AddExecutor实际上是往Repository里面AddItem，那么ItemAdded事件会被viewmodel响应，从而更新UI
 2. 不加新的数据结构，而是为AddExecutor产生新的事件ExecutorAdded。ViewModel中订阅此事件，从而在响应事件时更新UI。
 显然，我们不应该为了ViewModel而去改变Model，或者说尽量少改动。所以这里方案二明显较优</t>
+    </r>
+  </si>
+  <si>
+    <t>Assets Using Record</t>
+  </si>
+  <si>
+    <t>mainWindowViewModel到处都是，要不要弄成全局的？</t>
+  </si>
+  <si>
+    <r>
+      <t>在viewmodel中添加一个Save As命令，对应UI上一个按钮。按下这个按钮，即执行这个命令：
+1. 新建一个workspace，其model的值，是从原model深度复制过来的
+2. 将这个workspace添加到mainWindowViewModel
+这里引发一个问题(ID 11)是，workspace (Both All and single)需要“</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>知道</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>”mainWindowViewModel</t>
     </r>
   </si>
 </sst>
@@ -511,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -558,7 +593,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -572,15 +607,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="60">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30">
@@ -645,6 +683,25 @@
       </c>
       <c r="D10" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated IsNewBatteryType and CanSave
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -669,6 +669,9 @@
       </c>
       <c r="B9" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="210">

</xml_diff>